<commit_message>
Addressbook 경로 오류 수정
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uipathAdmin\OneDrive - Moedog, Inc\Workspace\UiPath\KakaoTalk\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uipathAdmin\Documents\COVD19KakaoTalk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189AA528-0A80-4B53-90A8-198BBCEFE6BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA05149-291B-4031-8E6C-C3FAEDF2747C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11130" yWindow="2977" windowWidth="28800" windowHeight="15593" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4777" yWindow="4777" windowWidth="28801" windowHeight="15473" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -270,9 +270,6 @@
     <t>Addressbook</t>
   </si>
   <si>
-    <t>Data\Addressbook.xlsx</t>
-  </si>
-  <si>
     <t>COVD19_Addressbook</t>
   </si>
   <si>
@@ -292,6 +289,10 @@
   </si>
   <si>
     <t xml:space="preserve">Forms or SurveyMonkey, 현재는 2개만 제공됨 </t>
+  </si>
+  <si>
+    <t>C:\Users\uipathAdmin\Documents\Addressbook.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -378,8 +379,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,7 +396,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -694,7 +695,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -849,18 +850,18 @@
         <v>81</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" t="s">
         <v>86</v>
-      </c>
-      <c r="C15" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -1860,7 +1861,7 @@
     <hyperlink ref="B13" r:id="rId2" xr:uid="{9B8D323F-0DB3-4B16-A228-35E8E3C66B8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3197,21 +3198,21 @@
         <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Multilanguage support feature added ( considering Config fist, if not specified at Config then see system's cultureinfo )
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uipathAdmin\Documents\UiPath\COVID19KakaoTalk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954DA666-3297-452C-8043-EAFA38EF3DA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FCDBC6-C7B5-4140-9D2C-9871AC74376B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3083" yWindow="2055" windowWidth="28800" windowHeight="15592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -204,28 +204,7 @@
     <t xml:space="preserve">http://bit.ly/2I34gLE </t>
   </si>
   <si>
-    <t>재전송 시간(전송후 n 시간 동안 답이 없으면 재전송 함)</t>
-  </si>
-  <si>
-    <t>응답을 볼수 있는 URL</t>
-  </si>
-  <si>
-    <t>직원이 답변할 URL</t>
-  </si>
-  <si>
-    <t>조직을 구분하는 구분자, 영문자2자와 하이튼, 예, UP-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">알림 메세지 포맷팅 문자를 넣은 경우 {0}은 이름, {1} 오늘날자, {2} 서베이 링크가 됨 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">회신이 없는 경우 재전송 알림 메세지 포맷팅 문자를 넣은 경우 {0}은 이름, {1} 오늘날자, {2} 서베이 링크가 됨 </t>
-  </si>
-  <si>
     <t>Addressbook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">직원 주소록 파일 </t>
   </si>
   <si>
     <t>SurveySite</t>
@@ -908,6 +887,42 @@
   </si>
   <si>
     <t xml:space="preserve">KakaoTalk,  Workplace, Whatsapp </t>
+  </si>
+  <si>
+    <t>ReportFinishColumnName</t>
+  </si>
+  <si>
+    <t>완료 시간</t>
+  </si>
+  <si>
+    <t>COVID19_ReportColumnName</t>
+  </si>
+  <si>
+    <t>Column name which says finished time</t>
+  </si>
+  <si>
+    <t>Addressbook file path, which contains column name as Name, PhoneNumber, ID, Status as Mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reminder message form , {0} for Name, {1} for Date, {2} for Survey link {3} for newline </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message form , {0} for Name, {1} for Date, {2} for Survey link {3} for newline </t>
+  </si>
+  <si>
+    <t>prefix for subgroup</t>
+  </si>
+  <si>
+    <t>Survey link which every employee can answer his/her health status</t>
+  </si>
+  <si>
+    <t>Suvey admin url which robot can access and download answers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interval time for reminder message, in hour </t>
+  </si>
+  <si>
+    <t>FinishTimeColumnName</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1346,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -1381,7 +1396,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1392,7 +1407,7 @@
         <v>47</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -1400,7 +1415,7 @@
         <v>55</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -1408,7 +1423,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -1419,7 +1434,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1435,10 +1450,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="33.75">
@@ -1446,7 +1461,7 @@
         <v>52</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="50.65">
@@ -1454,7 +1469,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1483,49 +1498,56 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3735,7 +3757,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -3784,10 +3806,10 @@
         <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3795,10 +3817,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3806,10 +3828,10 @@
         <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3817,10 +3839,10 @@
         <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3828,10 +3850,10 @@
         <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3839,46 +3861,56 @@
         <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
add multi-language execution environment consideration
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uipathAdmin\Documents\UiPath\COVID19KakaoTalk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FCDBC6-C7B5-4140-9D2C-9871AC74376B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F57516-C10A-4B68-9590-6E30B9138E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3083" yWindow="2055" windowWidth="28800" windowHeight="15592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="4470" windowWidth="19673" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -889,18 +889,6 @@
     <t xml:space="preserve">KakaoTalk,  Workplace, Whatsapp </t>
   </si>
   <si>
-    <t>ReportFinishColumnName</t>
-  </si>
-  <si>
-    <t>완료 시간</t>
-  </si>
-  <si>
-    <t>COVID19_ReportColumnName</t>
-  </si>
-  <si>
-    <t>Column name which says finished time</t>
-  </si>
-  <si>
     <t>Addressbook file path, which contains column name as Name, PhoneNumber, ID, Status as Mandatory</t>
   </si>
   <si>
@@ -920,9 +908,6 @@
   </si>
   <si>
     <t xml:space="preserve">interval time for reminder message, in hour </t>
-  </si>
-  <si>
-    <t>FinishTimeColumnName</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1331,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -1541,12 +1526,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>92</v>
-      </c>
+      <c r="A19" s="9"/>
+      <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3757,7 +3738,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -3809,7 +3790,7 @@
         <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3820,7 +3801,7 @@
         <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3831,7 +3812,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3842,7 +3823,7 @@
         <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3853,7 +3834,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3864,7 +3845,7 @@
         <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3875,7 +3856,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -3901,15 +3882,9 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="A11" s="9"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add new asset: ProgressMessageFormat Add new identical field for Addressbook and english form: Employee Email
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,24 +5,34 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uipathAdmin\Documents\UiPath\COVID19KakaoTalk\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoang Duong\Documents\UiPath\COVID19KakaoTalk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F57516-C10A-4B68-9590-6E30B9138E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7871927-2F82-4CE5-A581-022C79A1516D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="4470" windowWidth="19673" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27930" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -861,10 +871,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>COVID19_KakaoTalkQueue</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>COVID19_Kakao_Credential</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -886,9 +892,6 @@
     <t>KakaoTalk</t>
   </si>
   <si>
-    <t xml:space="preserve">KakaoTalk,  Workplace, Whatsapp </t>
-  </si>
-  <si>
     <t>Addressbook file path, which contains column name as Name, PhoneNumber, ID, Status as Mandatory</t>
   </si>
   <si>
@@ -908,13 +911,46 @@
   </si>
   <si>
     <t xml:space="preserve">interval time for reminder message, in hour </t>
+  </si>
+  <si>
+    <t>KakaoTalk,  Workplace, Whatsapp, WhatsappWeb</t>
+  </si>
+  <si>
+    <t>Locale</t>
+  </si>
+  <si>
+    <t>COVID19_Locale</t>
+  </si>
+  <si>
+    <t>en, ko</t>
+  </si>
+  <si>
+    <t>COVID19_ContactQueue</t>
+  </si>
+  <si>
+    <t>COVID19_ProgressMessageFormat</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[COVID19] {0}, {1} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>response request messages have been sent.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -959,6 +995,12 @@
       <family val="2"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF485056"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -987,7 +1029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1013,6 +1055,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1330,16 +1373,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="52.59765625" customWidth="1"/>
-    <col min="3" max="3" width="50.53125" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1380,8 +1423,8 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>83</v>
+      <c r="B2" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1392,7 +1435,7 @@
         <v>47</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -1400,7 +1443,7 @@
         <v>55</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -1408,7 +1451,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -1438,10 +1481,10 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="33.75">
+    <row r="9" spans="1:26" ht="49.5">
       <c r="A9" s="3" t="s">
         <v>52</v>
       </c>
@@ -1449,7 +1492,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="50.65">
+    <row r="10" spans="1:26" ht="49.5">
       <c r="A10" s="3" t="s">
         <v>56</v>
       </c>
@@ -1516,13 +1559,13 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
@@ -2524,14 +2567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.59765625" customWidth="1"/>
+    <col min="2" max="2" width="63.5703125" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3737,15 +3782,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.1328125" customWidth="1"/>
-    <col min="2" max="2" width="29.46484375" customWidth="1"/>
-    <col min="3" max="26" width="65.3984375" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3790,7 +3835,7 @@
         <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3801,7 +3846,7 @@
         <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3812,7 +3857,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3823,7 +3868,7 @@
         <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3834,7 +3879,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3845,7 +3890,7 @@
         <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3856,7 +3901,7 @@
         <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -3882,11 +3927,27 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
update locale related modification
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uipathAdmin\Documents\UiPath\COVID19KakaoTalk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F57516-C10A-4B68-9590-6E30B9138E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035AE0E1-E431-4A6E-9102-8893D66D8A31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="4470" windowWidth="19673" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7628" yWindow="2370" windowWidth="28800" windowHeight="15592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -204,7 +204,28 @@
     <t xml:space="preserve">http://bit.ly/2I34gLE </t>
   </si>
   <si>
+    <t>재전송 시간(전송후 n 시간 동안 답이 없으면 재전송 함)</t>
+  </si>
+  <si>
+    <t>응답을 볼수 있는 URL</t>
+  </si>
+  <si>
+    <t>직원이 답변할 URL</t>
+  </si>
+  <si>
+    <t>조직을 구분하는 구분자, 영문자2자와 하이튼, 예, UP-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">알림 메세지 포맷팅 문자를 넣은 경우 {0}은 이름, {1} 오늘날자, {2} 서베이 링크가 됨 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">회신이 없는 경우 재전송 알림 메세지 포맷팅 문자를 넣은 경우 {0}은 이름, {1} 오늘날자, {2} 서베이 링크가 됨 </t>
+  </si>
+  <si>
     <t>Addressbook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">직원 주소록 파일 </t>
   </si>
   <si>
     <t>SurveySite</t>
@@ -886,28 +907,7 @@
     <t>KakaoTalk</t>
   </si>
   <si>
-    <t xml:space="preserve">KakaoTalk,  Workplace, Whatsapp </t>
-  </si>
-  <si>
-    <t>Addressbook file path, which contains column name as Name, PhoneNumber, ID, Status as Mandatory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reminder message form , {0} for Name, {1} for Date, {2} for Survey link {3} for newline </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Message form , {0} for Name, {1} for Date, {2} for Survey link {3} for newline </t>
-  </si>
-  <si>
-    <t>prefix for subgroup</t>
-  </si>
-  <si>
-    <t>Survey link which every employee can answer his/her health status</t>
-  </si>
-  <si>
-    <t>Suvey admin url which robot can access and download answers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interval time for reminder message, in hour </t>
+    <t>KakaoTalk,  Workplace</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1331,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -1381,7 +1381,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1392,7 +1392,7 @@
         <v>47</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -1400,7 +1400,7 @@
         <v>55</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -1408,7 +1408,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -1419,7 +1419,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1435,10 +1435,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="33.75">
@@ -1446,7 +1446,7 @@
         <v>52</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="50.65">
@@ -1454,7 +1454,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1483,52 +1483,49 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="8"/>
-    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3738,7 +3735,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -3787,10 +3784,10 @@
         <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3798,10 +3795,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3809,10 +3806,10 @@
         <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3820,10 +3817,10 @@
         <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3831,10 +3828,10 @@
         <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3842,50 +3839,46 @@
         <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add SUMMARY_REPORTS command to send EOD reports (to configured email address on Assets)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoang Duong\Documents\UiPath\COVID19KakaoTalk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7871927-2F82-4CE5-A581-022C79A1516D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE46C00-E0E2-47A3-BF89-AB98CBAFCD0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27930" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27915" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="106">
   <si>
     <t>Name</t>
   </si>
@@ -944,6 +944,15 @@
       </rPr>
       <t>response request messages have been sent.</t>
     </r>
+  </si>
+  <si>
+    <t>COVID19_SummaryReportEmail</t>
+  </si>
+  <si>
+    <t>SummaryReportEmail</t>
+  </si>
+  <si>
+    <t>Email address to send summary reports at end of day (i.e. hr@corp.com)</t>
   </si>
 </sst>
 </file>
@@ -3783,7 +3792,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3948,7 +3957,17 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4939,5 +4958,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on adding summary report and send email to who is charging this job.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoang Duong\Documents\UiPath\COVID19KakaoTalk\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uipathAdmin\Documents\UiPath\COVID19KakaoTalk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE46C00-E0E2-47A3-BF89-AB98CBAFCD0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529F2EC6-844E-4FAE-821F-4B12A83C5EE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27915" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7988" yWindow="1125" windowWidth="29415" windowHeight="19703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -953,6 +953,20 @@
   </si>
   <si>
     <t>Email address to send summary reports at end of day (i.e. hr@corp.com)</t>
+  </si>
+  <si>
+    <t>SummaryReportFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0} 직원건강체크 결과입니다.
+전체 직원 : {1}명 
+응답한 직원: {2}명 
+1. 체온이 37.5도 이상인 직원 : 총 {3}명 
+{4}
+2. 현재 호흡기 증상이 있는 직원 : 총 {5}명 
+{6}
+이상입니다. 
+From Your UiPath Robot. </t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1052,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1065,6 +1079,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1382,16 +1399,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.73046875" customWidth="1"/>
+    <col min="2" max="2" width="52.59765625" customWidth="1"/>
+    <col min="3" max="3" width="50.59765625" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1493,7 +1510,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="49.5">
+    <row r="9" spans="1:26" ht="33.75">
       <c r="A9" s="3" t="s">
         <v>52</v>
       </c>
@@ -1501,7 +1518,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="49.5">
+    <row r="10" spans="1:26" ht="50.65">
       <c r="A10" s="3" t="s">
         <v>56</v>
       </c>
@@ -1581,7 +1598,14 @@
       <c r="A19" s="9"/>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="199.5">
+      <c r="A20" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2580,12 +2604,12 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.59765625" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3791,15 +3815,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.1328125" customWidth="1"/>
+    <col min="2" max="2" width="29.3984375" customWidth="1"/>
+    <col min="3" max="26" width="65.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>